<commit_message>
Added Encounter and related extensions. Updated profile page.
</commit_message>
<xml_diff>
--- a/docs/UKCore-List.xlsx
+++ b/docs/UKCore-List.xlsx
@@ -772,7 +772,7 @@
     <t>List.encounter</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Encounter)
+    <t xml:space="preserve">Reference(https://fhir.nhs.uk/R4/StructureDefinition/UKCore-Encounter)
 </t>
   </si>
   <si>
@@ -975,7 +975,7 @@
     <t>List.note.author[x]</t>
   </si>
   <si>
-    <t>Reference(RelatedPerson|https://fhir.nhs.uk/R4/StructureDefinition/UKCore-Patient|https://fhir.nhs.uk/R4/StructureDefinition/UKCore-Organization|https://fhir.nhs.uk/R4/StructureDefinition/UKCore-Practitioner)
+    <t>Reference(https://fhir.nhs.uk/R4/StructureDefinition/UKCore-Patient|https://fhir.nhs.uk/R4/StructureDefinition/UKCore-Organization|https://fhir.nhs.uk/R4/StructureDefinition/UKCore-Practitioner|https://fhir.nhs.uk/R4/StructureDefinition/UKCore-RelatedPerson)
 string</t>
   </si>
   <si>

</xml_diff>